<commit_message>
changed to 4 quarter system
</commit_message>
<xml_diff>
--- a/wdhoy/financial_cleaned.xlsx
+++ b/wdhoy/financial_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuang/code/revenue-forecast-analysis/wdhoy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DED3A9-2F5B-8A49-84D0-163CE626ED93}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B47808-A4FB-5143-989E-5B59E481A354}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,7 +695,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,6 +723,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -868,6 +886,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1210,10 +1237,10 @@
   <dimension ref="A1:CC72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AV6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BJ16" sqref="BJ16"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -1961,197 +1988,197 @@
       <c r="BZ8" s="72"/>
       <c r="CC8" s="72"/>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.15">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:81" s="78" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="78" t="s">
         <v>111</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="79">
         <v>316489</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="80">
         <f>E9/E16</f>
         <v>0.13992100488436332</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4">
+      <c r="G9" s="79"/>
+      <c r="H9" s="79">
         <v>329889</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="80">
         <f>H9/H16</f>
         <v>0.14086503151314328</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4">
+      <c r="J9" s="79"/>
+      <c r="K9" s="79">
         <v>320117</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="80">
         <f>K9/K16</f>
         <v>0.15106064803039362</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4">
+      <c r="M9" s="79"/>
+      <c r="N9" s="79">
         <v>477794</v>
       </c>
-      <c r="O9" s="28">
+      <c r="O9" s="80">
         <f>N9/N16</f>
         <v>0.17832013456658669</v>
       </c>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4">
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79">
         <v>457870</v>
       </c>
-      <c r="R9" s="28">
+      <c r="R9" s="80">
         <f>Q9/Q16</f>
         <v>0.17693277621039183</v>
       </c>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4">
+      <c r="S9" s="79"/>
+      <c r="T9" s="79">
         <v>390262</v>
       </c>
-      <c r="U9" s="28">
+      <c r="U9" s="80">
         <f>T9/T16</f>
         <v>0.17264303605286233</v>
       </c>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4">
+      <c r="V9" s="79"/>
+      <c r="W9" s="79">
         <v>467795</v>
       </c>
-      <c r="X9" s="28">
+      <c r="X9" s="80">
         <f>W9/W16</f>
         <v>0.16861001578708343</v>
       </c>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4">
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="79">
         <v>437050</v>
       </c>
-      <c r="AA9" s="28">
+      <c r="AA9" s="80">
         <f>Z9/Z16</f>
         <v>0.15846605008549661</v>
       </c>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4">
+      <c r="AB9" s="79"/>
+      <c r="AC9" s="79">
         <v>427650</v>
       </c>
-      <c r="AD9" s="28">
+      <c r="AD9" s="80">
         <f>AC9/AC16</f>
         <v>0.16432617622037116</v>
       </c>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="4">
+      <c r="AE9" s="79"/>
+      <c r="AF9" s="79">
         <v>490659</v>
       </c>
-      <c r="AG9" s="28">
+      <c r="AG9" s="80">
         <f>AF9/AF16</f>
         <v>0.1481880257573337</v>
       </c>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="4">
+      <c r="AH9" s="79"/>
+      <c r="AI9" s="79">
         <v>474907</v>
       </c>
-      <c r="AJ9" s="28">
+      <c r="AJ9" s="80">
         <f>AI9/AI16</f>
         <v>0.146325494091606</v>
       </c>
-      <c r="AL9" s="4">
+      <c r="AL9" s="79">
         <v>437272</v>
       </c>
-      <c r="AM9" s="28">
+      <c r="AM9" s="80">
         <f>AL9/AL16</f>
         <v>0.14866082796430416</v>
       </c>
-      <c r="AO9" s="4">
+      <c r="AO9" s="79">
         <v>545245</v>
       </c>
-      <c r="AP9" s="28">
+      <c r="AP9" s="80">
         <f>AO9/AO16</f>
         <v>0.14539106756020218</v>
       </c>
-      <c r="AQ9" s="4"/>
-      <c r="AR9" s="4">
+      <c r="AQ9" s="79"/>
+      <c r="AR9" s="79">
         <v>530270</v>
       </c>
-      <c r="AS9" s="28">
+      <c r="AS9" s="80">
         <f>AR9/AR16</f>
         <v>0.14733020781875053</v>
       </c>
-      <c r="AU9" s="4">
+      <c r="AU9" s="79">
         <v>481676</v>
       </c>
-      <c r="AV9" s="28">
+      <c r="AV9" s="80">
         <f>AU9/AU16</f>
         <v>0.14145165941606364</v>
       </c>
-      <c r="AX9" s="4">
+      <c r="AX9" s="79">
         <v>576625</v>
       </c>
-      <c r="AY9" s="28">
+      <c r="AY9" s="80">
         <f>AX9/AX16</f>
         <v>0.1436216900695611</v>
       </c>
-      <c r="AZ9" s="4"/>
-      <c r="BA9" s="4">
+      <c r="AZ9" s="79"/>
+      <c r="BA9" s="79">
         <v>591774</v>
       </c>
-      <c r="BB9" s="28">
+      <c r="BB9" s="80">
         <f>BA9/BA16</f>
         <v>0.15232619108844908</v>
       </c>
-      <c r="BD9" s="4">
+      <c r="BD9" s="79">
         <v>513796</v>
       </c>
-      <c r="BE9" s="28">
+      <c r="BE9" s="80">
         <f>BD9/BD16</f>
         <v>0.14497347540355451</v>
       </c>
-      <c r="BG9" s="4">
+      <c r="BG9" s="79">
         <v>567741</v>
       </c>
-      <c r="BH9" s="28">
+      <c r="BH9" s="80">
         <f>BG9/BG16</f>
         <v>0.13758795226622036</v>
       </c>
-      <c r="BI9" s="4"/>
-      <c r="BJ9" s="4">
+      <c r="BI9" s="79"/>
+      <c r="BJ9" s="79">
         <v>560402</v>
       </c>
-      <c r="BK9" s="28">
+      <c r="BK9" s="80">
         <f>BJ9/BJ16</f>
         <v>0.14019695550538772</v>
       </c>
-      <c r="BM9" s="4">
+      <c r="BM9" s="79">
         <v>488385</v>
       </c>
-      <c r="BN9" s="28">
+      <c r="BN9" s="80">
         <f>BM9/BM16</f>
         <v>0.13194160027059124</v>
       </c>
-      <c r="BP9" s="4">
+      <c r="BP9" s="79">
         <v>553390.15700000001</v>
       </c>
-      <c r="BQ9" s="28">
+      <c r="BQ9" s="80">
         <f>BP9/BP16</f>
         <v>0.12182948406723623</v>
       </c>
-      <c r="BR9" s="4"/>
-      <c r="BS9" s="4">
+      <c r="BR9" s="79"/>
+      <c r="BS9" s="79">
         <v>547767</v>
       </c>
-      <c r="BT9" s="28">
+      <c r="BT9" s="80">
         <f>BS9/BS16</f>
         <v>0.12487165575474624</v>
       </c>
-      <c r="BU9" s="4"/>
-      <c r="BV9" s="4">
+      <c r="BU9" s="79"/>
+      <c r="BV9" s="79">
         <v>552755</v>
       </c>
-      <c r="BW9" s="28">
+      <c r="BW9" s="80">
         <f>BV9/BV16</f>
         <v>0.13458795032988663</v>
       </c>
-      <c r="BY9" s="4"/>
-      <c r="BZ9" s="28"/>
-      <c r="CB9" s="4"/>
-      <c r="CC9" s="28"/>
+      <c r="BY9" s="79"/>
+      <c r="BZ9" s="80"/>
+      <c r="CB9" s="79"/>
+      <c r="CC9" s="80"/>
     </row>
     <row r="10" spans="1:81" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
@@ -2613,221 +2640,221 @@
       <c r="CB13" s="5"/>
       <c r="CC13" s="28"/>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.15">
-      <c r="C14" s="1" t="s">
+    <row r="14" spans="1:81" s="81" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C14" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="82">
         <f>SUM(E11:E13)</f>
         <v>113357</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="83">
         <f>E14/E16</f>
         <v>5.0115565945978449E-2</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4">
+      <c r="G14" s="82"/>
+      <c r="H14" s="82">
         <f>SUM(H11:H13)</f>
         <v>122393</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="83">
         <f>H14/H16</f>
         <v>5.2262712009155041E-2</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4">
+      <c r="J14" s="82"/>
+      <c r="K14" s="82">
         <f>SUM(K11:K13)</f>
         <v>110543</v>
       </c>
-      <c r="L14" s="28">
+      <c r="L14" s="83">
         <f>K14/K16</f>
         <v>5.216435620483699E-2</v>
       </c>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4">
+      <c r="M14" s="82"/>
+      <c r="N14" s="82">
         <f>SUM(N11:N13)</f>
         <v>130083</v>
       </c>
-      <c r="O14" s="28">
+      <c r="O14" s="83">
         <f>N14/N16</f>
         <v>4.8548994053557171E-2</v>
       </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4">
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82">
         <f>SUM(Q11:Q13)</f>
         <v>114966</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14" s="83">
         <f>Q14/Q16</f>
         <v>4.4425827308633252E-2</v>
       </c>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4">
+      <c r="S14" s="82"/>
+      <c r="T14" s="82">
         <f>SUM(T11:T13)</f>
         <v>103562</v>
       </c>
-      <c r="U14" s="28">
+      <c r="U14" s="83">
         <f>T14/T16</f>
         <v>4.5813474280628208E-2</v>
       </c>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4">
+      <c r="V14" s="82"/>
+      <c r="W14" s="82">
         <f>SUM(W11:W13)</f>
         <v>117718</v>
       </c>
-      <c r="X14" s="28">
+      <c r="X14" s="83">
         <f>W14/W16</f>
         <v>4.2429769104893995E-2</v>
       </c>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4">
+      <c r="Y14" s="82"/>
+      <c r="Z14" s="82">
         <f>SUM(Z11:Z13)</f>
         <v>128990</v>
       </c>
-      <c r="AA14" s="28">
+      <c r="AA14" s="83">
         <f>Z14/Z16</f>
         <v>4.6769330283784938E-2</v>
       </c>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4">
+      <c r="AB14" s="82"/>
+      <c r="AC14" s="82">
         <f>SUM(AC11:AC13)</f>
         <v>106054</v>
       </c>
-      <c r="AD14" s="28">
+      <c r="AD14" s="83">
         <f>AC14/AC16</f>
         <v>4.0751662090202832E-2</v>
       </c>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4">
+      <c r="AE14" s="82"/>
+      <c r="AF14" s="82">
         <f>SUM(AF11:AF13)</f>
         <v>118643</v>
       </c>
-      <c r="AG14" s="28">
+      <c r="AG14" s="83">
         <f>AF14/AF16</f>
         <v>3.5832364106084549E-2</v>
       </c>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="4">
+      <c r="AH14" s="82"/>
+      <c r="AI14" s="82">
         <f>SUM(AI11:AI13)</f>
         <v>131122</v>
       </c>
-      <c r="AJ14" s="28">
+      <c r="AJ14" s="83">
         <f>AI14/AI16</f>
         <v>4.0400523547304126E-2</v>
       </c>
-      <c r="AL14" s="4">
+      <c r="AL14" s="82">
         <f>SUM(AL11:AL13)</f>
         <v>107295</v>
       </c>
-      <c r="AM14" s="28">
+      <c r="AM14" s="83">
         <f>AL14/AL16</f>
         <v>3.6477440898182403E-2</v>
       </c>
-      <c r="AO14" s="4">
+      <c r="AO14" s="82">
         <f>SUM(AO11:AO13)</f>
         <v>144610</v>
       </c>
-      <c r="AP14" s="28">
+      <c r="AP14" s="83">
         <f>AO14/AO16</f>
         <v>3.8560651229962384E-2</v>
       </c>
-      <c r="AQ14" s="4"/>
-      <c r="AR14" s="4">
+      <c r="AQ14" s="82"/>
+      <c r="AR14" s="82">
         <f>SUM(AR11:AR13)</f>
         <v>148759</v>
       </c>
-      <c r="AS14" s="28">
+      <c r="AS14" s="83">
         <f>AR14/AR16</f>
         <v>4.1331198040450171E-2</v>
       </c>
-      <c r="AU14" s="4">
+      <c r="AU14" s="82">
         <f>SUM(AU11:AU13)</f>
         <v>129043</v>
       </c>
-      <c r="AV14" s="28">
+      <c r="AV14" s="83">
         <f>AU14/AU16</f>
         <v>3.789548677124685E-2</v>
       </c>
-      <c r="AX14" s="4">
+      <c r="AX14" s="82">
         <f>SUM(AX11:AX13)</f>
         <v>145605</v>
       </c>
-      <c r="AY14" s="28">
+      <c r="AY14" s="83">
         <f>AX14/AX16</f>
         <v>3.6266266954395741E-2</v>
       </c>
-      <c r="AZ14" s="4"/>
-      <c r="BA14" s="4">
+      <c r="AZ14" s="82"/>
+      <c r="BA14" s="82">
         <f>SUM(BA11:BA13)</f>
         <v>142919</v>
       </c>
-      <c r="BB14" s="28">
+      <c r="BB14" s="83">
         <f>BA14/BA16</f>
         <v>3.6788211216055543E-2</v>
       </c>
-      <c r="BD14" s="4">
+      <c r="BD14" s="82">
         <f>SUM(BD11:BD13)</f>
         <v>121310</v>
       </c>
-      <c r="BE14" s="28">
+      <c r="BE14" s="83">
         <f>BD14/BD16</f>
         <v>3.4229017550166205E-2</v>
       </c>
-      <c r="BG14" s="4">
+      <c r="BG14" s="82">
         <f>SUM(BG11:BG13)</f>
         <v>129671</v>
       </c>
-      <c r="BH14" s="28">
+      <c r="BH14" s="83">
         <f>BG14/BG16</f>
         <v>3.1424835194768498E-2</v>
       </c>
-      <c r="BI14" s="4"/>
-      <c r="BJ14" s="4">
+      <c r="BI14" s="82"/>
+      <c r="BJ14" s="82">
         <f>SUM(BJ11:BJ13)</f>
         <v>136032</v>
       </c>
-      <c r="BK14" s="28">
+      <c r="BK14" s="83">
         <f>BJ14/BJ16</f>
         <v>3.4031413612565446E-2</v>
       </c>
-      <c r="BM14" s="4">
+      <c r="BM14" s="82">
         <f>SUM(BM11:BM13)</f>
         <v>122526</v>
       </c>
-      <c r="BN14" s="28">
+      <c r="BN14" s="83">
         <f>BM14/BM16</f>
         <v>3.3101500895306904E-2</v>
       </c>
-      <c r="BP14" s="4">
+      <c r="BP14" s="82">
         <f>SUM(BP11:BP13)</f>
         <v>145570.05900000001</v>
       </c>
-      <c r="BQ14" s="28">
+      <c r="BQ14" s="83">
         <f>BP14/BP16</f>
         <v>3.2047417105771074E-2</v>
       </c>
-      <c r="BR14" s="4"/>
-      <c r="BS14" s="4">
+      <c r="BR14" s="82"/>
+      <c r="BS14" s="82">
         <f>SUM(BS11:BS13)</f>
         <v>144673</v>
       </c>
-      <c r="BT14" s="28">
+      <c r="BT14" s="83">
         <f>BS14/BS16</f>
         <v>3.2980367661809493E-2</v>
       </c>
-      <c r="BU14" s="4"/>
-      <c r="BV14" s="4">
+      <c r="BU14" s="82"/>
+      <c r="BV14" s="82">
         <f>SUM(BV11:BV13)</f>
         <v>128722</v>
       </c>
-      <c r="BW14" s="28">
+      <c r="BW14" s="83">
         <f>BV14/BV16</f>
         <v>3.1341969122601634E-2</v>
       </c>
-      <c r="BY14" s="4"/>
-      <c r="BZ14" s="28"/>
-      <c r="CB14" s="4"/>
-      <c r="CC14" s="28"/>
+      <c r="BY14" s="82"/>
+      <c r="BZ14" s="83"/>
+      <c r="CB14" s="82"/>
+      <c r="CC14" s="83"/>
     </row>
     <row r="15" spans="1:81" x14ac:dyDescent="0.15">
       <c r="E15" s="5"/>
@@ -2898,221 +2925,221 @@
       <c r="CB15" s="5"/>
       <c r="CC15" s="29"/>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:81" s="75" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="76">
         <f>+E8+E9+E14</f>
         <v>2261912</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="77">
         <f>E16/E16</f>
         <v>1</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4">
+      <c r="G16" s="76"/>
+      <c r="H16" s="76">
         <f>+H8+H9+H14</f>
         <v>2341880</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="77">
         <f>H16/H16</f>
         <v>1</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4">
+      <c r="J16" s="76"/>
+      <c r="K16" s="76">
         <f>+K8+K9+K14</f>
         <v>2119129</v>
       </c>
-      <c r="L16" s="28">
+      <c r="L16" s="77">
         <f>K16/K16</f>
         <v>1</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4">
+      <c r="M16" s="76"/>
+      <c r="N16" s="76">
         <f>+N8+N9+N14</f>
         <v>2679417</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="77">
         <f>N16/N16</f>
         <v>1</v>
       </c>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4">
+      <c r="P16" s="76"/>
+      <c r="Q16" s="76">
         <f>+Q8+Q9+Q14</f>
         <v>2587819</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16" s="77">
         <f>Q16/Q16</f>
         <v>1</v>
       </c>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4">
+      <c r="S16" s="76"/>
+      <c r="T16" s="76">
         <f>+T8+T9+T14</f>
         <v>2260514</v>
       </c>
-      <c r="U16" s="28">
+      <c r="U16" s="77">
         <f>T16/T16</f>
         <v>1</v>
       </c>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4">
+      <c r="V16" s="76"/>
+      <c r="W16" s="76">
         <f>+W8+W9+W14</f>
         <v>2774420</v>
       </c>
-      <c r="X16" s="28">
+      <c r="X16" s="77">
         <f>W16/W16</f>
         <v>1</v>
       </c>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4">
+      <c r="Y16" s="76"/>
+      <c r="Z16" s="76">
         <f>+Z8+Z9+Z14</f>
         <v>2758004</v>
       </c>
-      <c r="AA16" s="28">
+      <c r="AA16" s="77">
         <f>Z16/Z16</f>
         <v>1</v>
       </c>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4">
+      <c r="AB16" s="76"/>
+      <c r="AC16" s="76">
         <f>+AC8+AC9+AC14</f>
         <v>2602446</v>
       </c>
-      <c r="AD16" s="28">
+      <c r="AD16" s="77">
         <f>AC16/AC16</f>
         <v>1</v>
       </c>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4">
+      <c r="AE16" s="76"/>
+      <c r="AF16" s="76">
         <f>+AF8+AF9+AF14</f>
         <v>3311057</v>
       </c>
-      <c r="AG16" s="28">
+      <c r="AG16" s="77">
         <f>AF16/AF16</f>
         <v>1</v>
       </c>
-      <c r="AH16" s="4"/>
-      <c r="AI16" s="4">
+      <c r="AH16" s="76"/>
+      <c r="AI16" s="76">
         <f>+AI8+AI9+AI14</f>
         <v>3245552</v>
       </c>
-      <c r="AJ16" s="28">
+      <c r="AJ16" s="77">
         <f>AI16/AI16</f>
         <v>1</v>
       </c>
-      <c r="AL16" s="4">
+      <c r="AL16" s="76">
         <f>+AL8+AL9+AL14</f>
         <v>2941407</v>
       </c>
-      <c r="AM16" s="28">
+      <c r="AM16" s="77">
         <f>AL16/AL16</f>
         <v>1</v>
       </c>
-      <c r="AO16" s="4">
+      <c r="AO16" s="76">
         <f>+AO8+AO9+AO14</f>
         <v>3750196</v>
       </c>
-      <c r="AP16" s="28">
+      <c r="AP16" s="77">
         <f>AO16/AO16</f>
         <v>1</v>
       </c>
-      <c r="AQ16" s="4"/>
-      <c r="AR16" s="4">
+      <c r="AQ16" s="76"/>
+      <c r="AR16" s="76">
         <f>+AR8+AR9+AR14</f>
         <v>3599194</v>
       </c>
-      <c r="AS16" s="28">
+      <c r="AS16" s="77">
         <f>AR16/AR16</f>
         <v>1</v>
       </c>
-      <c r="AU16" s="4">
+      <c r="AU16" s="76">
         <f>+AU8+AU9+AU14</f>
         <v>3405234</v>
       </c>
-      <c r="AV16" s="28">
+      <c r="AV16" s="77">
         <f>AU16/AU16</f>
         <v>1</v>
       </c>
-      <c r="AX16" s="4">
+      <c r="AX16" s="76">
         <f>+AX8+AX9+AX14</f>
         <v>4014888</v>
       </c>
-      <c r="AY16" s="28">
+      <c r="AY16" s="77">
         <f>AX16/AX16</f>
         <v>1</v>
       </c>
-      <c r="AZ16" s="4"/>
-      <c r="BA16" s="4">
+      <c r="AZ16" s="76"/>
+      <c r="BA16" s="76">
         <f>+BA8+BA9+BA14</f>
         <v>3884913</v>
       </c>
-      <c r="BB16" s="28">
+      <c r="BB16" s="77">
         <f>BA16/BA16</f>
         <v>1</v>
       </c>
-      <c r="BD16" s="4">
+      <c r="BD16" s="76">
         <f>+BD8+BD9+BD14</f>
         <v>3544069</v>
       </c>
-      <c r="BE16" s="28">
+      <c r="BE16" s="77">
         <f>BD16/BD16</f>
         <v>1</v>
       </c>
-      <c r="BG16" s="4">
+      <c r="BG16" s="76">
         <f>+BG8+BG9+BG14</f>
         <v>4126386</v>
       </c>
-      <c r="BH16" s="28">
+      <c r="BH16" s="77">
         <f>BG16/BG16</f>
         <v>1</v>
       </c>
-      <c r="BI16" s="4"/>
-      <c r="BJ16" s="4">
+      <c r="BI16" s="76"/>
+      <c r="BJ16" s="76">
         <f>+BJ8+BJ9+BJ14</f>
         <v>3997248</v>
       </c>
-      <c r="BK16" s="28">
+      <c r="BK16" s="77">
         <f>BJ16/BJ16</f>
         <v>1</v>
       </c>
-      <c r="BM16" s="4">
+      <c r="BM16" s="76">
         <f>+BM8+BM9+BM14</f>
         <v>3701524</v>
       </c>
-      <c r="BN16" s="28">
+      <c r="BN16" s="77">
         <f>BM16/BM16</f>
         <v>1</v>
       </c>
-      <c r="BP16" s="4">
+      <c r="BP16" s="76">
         <f>+BP8+BP9+BP14</f>
         <v>4542333.5839999998</v>
       </c>
-      <c r="BQ16" s="28">
+      <c r="BQ16" s="77">
         <f>BP16/BP16</f>
         <v>1</v>
       </c>
-      <c r="BR16" s="4"/>
-      <c r="BS16" s="4">
+      <c r="BR16" s="76"/>
+      <c r="BS16" s="76">
         <f>+BS8+BS9+BS14</f>
         <v>4386640</v>
       </c>
-      <c r="BT16" s="28">
+      <c r="BT16" s="77">
         <f>BS16/BS16</f>
         <v>1</v>
       </c>
-      <c r="BU16" s="4"/>
-      <c r="BV16" s="4">
+      <c r="BU16" s="76"/>
+      <c r="BV16" s="76">
         <f>+BV8+BV9+BV14</f>
         <v>4107017</v>
       </c>
-      <c r="BW16" s="28">
+      <c r="BW16" s="77">
         <f>BV16/BV16</f>
         <v>1</v>
       </c>
-      <c r="BY16" s="4"/>
-      <c r="BZ16" s="28"/>
-      <c r="CB16" s="4"/>
-      <c r="CC16" s="28"/>
+      <c r="BY16" s="76"/>
+      <c r="BZ16" s="77"/>
+      <c r="CB16" s="76"/>
+      <c r="CC16" s="77"/>
     </row>
     <row r="17" spans="1:81" x14ac:dyDescent="0.15">
       <c r="E17" s="4"/>

</xml_diff>